<commit_message>
lab excel pivot tables vs formulas
</commit_message>
<xml_diff>
--- a/your-code/PivotTable vs Formula Exercise.xlsx
+++ b/your-code/PivotTable vs Formula Exercise.xlsx
@@ -1,29 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c646aa9d978bc39d/Documents/Module 4/Week 1/Day 2 - Excel Pivot Tables and Macros/Lab/lab_2_Pivot-tables_vs_formulas/your-code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4f43df6d9434f4e/Ironhack/Module3/labs/lab-excel-pivot-tables-vs-formulas/your-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A3A7DBBF-F3AC-4897-BE43-8F94BEB89478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7683A57F-D9F9-4F18-9995-6F2FB9CE459C}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{A3A7DBBF-F3AC-4897-BE43-8F94BEB89478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0369F9D-91B3-9842-A7DA-C218983E5DC9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="3" r:id="rId1"/>
-    <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="Pivot" sheetId="4" r:id="rId2"/>
+    <sheet name="data" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$E$39</definedName>
-    <definedName name="ARTÍCULOS" localSheetId="1">data!$A$1:$E$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">data!$A$1:$E$39</definedName>
+    <definedName name="ARTÍCULOS" localSheetId="2">data!$A$1:$E$38</definedName>
     <definedName name="ARTÍCULOS">#REF!</definedName>
     <definedName name="data">data!$A$1:$E$39</definedName>
     <definedName name="miLista">data!$A$1:$E$4500</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="59" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="77">
   <si>
     <t>China</t>
   </si>
@@ -230,16 +234,59 @@
   </si>
   <si>
     <t>Lamp Base</t>
+  </si>
+  <si>
+    <t>Zeilenbeschriftungen</t>
+  </si>
+  <si>
+    <t>Spaltenbeschriftungen</t>
+  </si>
+  <si>
+    <t>Sum of Price</t>
+  </si>
+  <si>
+    <t>Count of Price</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Gesamt: Sum of Price</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Gesamt: Count of Price</t>
+  </si>
+  <si>
+    <t>Ceramics</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>Toys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Total </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00[$€]_-;\-* #,##0.00[$€]_-;_-* &quot;-&quot;??[$€]_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -303,7 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -327,12 +374,116 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="28">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -397,6 +548,516 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Fee Pieper" refreshedDate="45819.595366782407" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="38" xr:uid="{2A737C14-CBE3-F54B-B538-05FAF1C9EF50}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:F39" sheet="data"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Section" numFmtId="0">
+      <sharedItems count="5">
+        <s v="CERAMICS"/>
+        <s v="CLOTHING"/>
+        <s v="SPORTS"/>
+        <s v="HARDWARE"/>
+        <s v="TOYS"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Item" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2018-05-12T00:00:00" maxDate="2019-01-30T00:00:00"/>
+    </cacheField>
+    <cacheField name="Country" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Price" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.6060726263026939" maxValue="1254.4805452381811"/>
+    </cacheField>
+    <cacheField name="Year" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2018" maxValue="2019" count="2">
+        <n v="2019"/>
+        <n v="2018"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="38">
+  <r>
+    <x v="0"/>
+    <s v="Pipes"/>
+    <d v="2019-01-27T00:00:00"/>
+    <s v="China"/>
+    <n v="140.35435673674468"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Decorative Plate"/>
+    <d v="2018-12-24T00:00:00"/>
+    <s v="China"/>
+    <n v="45.07590782878367"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Tea Set"/>
+    <d v="2019-01-15T00:00:00"/>
+    <s v="China"/>
+    <n v="36.06"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Ashtray"/>
+    <d v="2018-05-12T00:00:00"/>
+    <s v="Japan"/>
+    <n v="16.45571141802796"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Flower Pot"/>
+    <d v="2019-01-05T00:00:00"/>
+    <s v="Spain"/>
+    <n v="24.202757443534914"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="China Pitcher"/>
+    <d v="2018-11-23T00:00:00"/>
+    <s v="China"/>
+    <n v="106.47530441263088"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Men's Card"/>
+    <d v="2018-10-23T00:00:00"/>
+    <s v="Italy"/>
+    <n v="237.14735614775282"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Women's Pants"/>
+    <d v="2018-09-10T00:00:00"/>
+    <s v="Morocco"/>
+    <n v="145.19250417703412"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Men's Shirt"/>
+    <d v="2019-01-07T00:00:00"/>
+    <s v="Spain"/>
+    <n v="55.94220667604246"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Women's Blouse"/>
+    <d v="2018-12-20T00:00:00"/>
+    <s v="China"/>
+    <n v="84.213816066255575"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Leather Jacket"/>
+    <d v="2018-09-09T00:00:00"/>
+    <s v="Italy"/>
+    <n v="435.5775125311024"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Men's Coat"/>
+    <d v="2019-01-14T00:00:00"/>
+    <s v="Italy"/>
+    <n v="203.268303823639"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Women's Coat"/>
+    <d v="2019-01-29T00:00:00"/>
+    <s v="Morocco"/>
+    <n v="300.06130323464714"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Leather Belt"/>
+    <d v="2019-01-03T00:00:00"/>
+    <s v="Spain"/>
+    <n v="3.6060726263026939"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Tennis Racket"/>
+    <d v="2018-09-14T00:00:00"/>
+    <s v="USA"/>
+    <n v="77.891168728138183"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Tracksuit"/>
+    <d v="2018-08-16T00:00:00"/>
+    <s v="USA"/>
+    <n v="193.39367494861347"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Electric Train"/>
+    <d v="2018-07-03T00:00:00"/>
+    <s v="Japan"/>
+    <n v="1254.4805452381811"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Olympic Pistol"/>
+    <d v="2019-01-04T00:00:00"/>
+    <s v="Sweden"/>
+    <n v="38.945584364069092"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Skateboard"/>
+    <d v="2019-01-21T00:00:00"/>
+    <s v="Morocco"/>
+    <n v="93.036673758609496"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Basketball"/>
+    <d v="2019-01-16T00:00:00"/>
+    <s v="Japan"/>
+    <n v="62.727633334535362"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Soccer Ball"/>
+    <d v="2018-12-08T00:00:00"/>
+    <s v="Spain"/>
+    <n v="36.595627035928501"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Sweatshirt"/>
+    <d v="2018-12-12T00:00:00"/>
+    <s v="USA"/>
+    <n v="365.98031084346042"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Mountain Bike"/>
+    <d v="2018-11-07T00:00:00"/>
+    <s v="USA"/>
+    <n v="470.41818422223025"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Screwdriver"/>
+    <d v="2018-10-05T00:00:00"/>
+    <s v="Spain"/>
+    <n v="5.5233012392869592"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Handsaw"/>
+    <d v="2018-10-28T00:00:00"/>
+    <s v="France"/>
+    <n v="25.170386931592802"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Wrench"/>
+    <d v="2019-01-15T00:00:00"/>
+    <s v="USA"/>
+    <n v="20.332239491303355"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Pliers"/>
+    <d v="2019-01-26T00:00:00"/>
+    <s v="Italy"/>
+    <n v="5.613453054944527"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Hammer"/>
+    <d v="2018-10-17T00:00:00"/>
+    <s v="Spain"/>
+    <n v="9.4959912492637599"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Screwdriver"/>
+    <d v="2019-01-18T00:00:00"/>
+    <s v="France"/>
+    <n v="7.5487120310603055"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Large File"/>
+    <d v="2018-11-19T00:00:00"/>
+    <s v="Spain"/>
+    <n v="18.390970394143739"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Drill Bit Set"/>
+    <d v="2018-11-06T00:00:00"/>
+    <s v="Taiwan"/>
+    <n v="12.579183344752563"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Remote Control Car"/>
+    <d v="2018-12-07T00:00:00"/>
+    <s v="Morocco"/>
+    <n v="132.87175603716659"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Walker"/>
+    <d v="2018-12-14T00:00:00"/>
+    <s v="Japan"/>
+    <n v="86.113014316108334"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Video Game Console"/>
+    <d v="2019-01-19T00:00:00"/>
+    <s v="USA"/>
+    <n v="368.78703737093264"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Walking Doll"/>
+    <d v="2018-10-14T00:00:00"/>
+    <s v="Spain"/>
+    <n v="87.549433245585561"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Soldier Fort"/>
+    <d v="2018-10-09T00:00:00"/>
+    <s v="Japan"/>
+    <n v="119.75166179846862"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Sound Gun"/>
+    <d v="2018-08-05T00:00:00"/>
+    <s v="Spain"/>
+    <n v="47.708340845984637"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Lamp Base"/>
+    <d v="2018-06-06T00:00:00"/>
+    <s v="Turkey"/>
+    <n v="33.133797314677921"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3C0F2A74-CFC4-A04B-8E4D-C3F64A2412DA}" name="PivotTable10" cacheId="59" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Grand Total" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:G11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="5"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Price" fld="4" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="Count of Price" fld="4" subtotal="count" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="7">
+    <format dxfId="27">
+      <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea field="5" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -688,38 +1349,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68408F57-2609-4CF7-9328-02FE8121296B}">
   <dimension ref="A2:A8"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="12" t="s">
         <v>11</v>
       </c>
@@ -731,35 +1392,352 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8554925C-1C01-8C4F-8834-DD786DCBE0BE}">
+  <dimension ref="A3:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="209" zoomScaleNormal="209" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="25.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.19921875" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.19921875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.3984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="25" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="26" max="38" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7">
+      <c r="B3" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" s="12">
+        <v>2018</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4">
+        <v>2019</v>
+      </c>
+      <c r="F4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="17">
+        <v>168.00692365944252</v>
+      </c>
+      <c r="C6" s="18">
+        <v>3</v>
+      </c>
+      <c r="D6" s="14">
+        <v>200.6171141802796</v>
+      </c>
+      <c r="E6" s="19">
+        <v>3</v>
+      </c>
+      <c r="F6" s="14">
+        <v>368.62403783972212</v>
+      </c>
+      <c r="G6" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="17">
+        <v>902.13118892214493</v>
+      </c>
+      <c r="C7" s="18">
+        <v>4</v>
+      </c>
+      <c r="D7" s="14">
+        <v>562.87788636063124</v>
+      </c>
+      <c r="E7" s="19">
+        <v>4</v>
+      </c>
+      <c r="F7" s="14">
+        <v>1465.0090752827762</v>
+      </c>
+      <c r="G7" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="17">
+        <v>71.15983315903982</v>
+      </c>
+      <c r="C8" s="18">
+        <v>5</v>
+      </c>
+      <c r="D8" s="14">
+        <v>33.494404577308188</v>
+      </c>
+      <c r="E8" s="19">
+        <v>3</v>
+      </c>
+      <c r="F8" s="14">
+        <v>104.65423773634801</v>
+      </c>
+      <c r="G8" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="17">
+        <v>2398.7595110165521</v>
+      </c>
+      <c r="C9" s="18">
+        <v>6</v>
+      </c>
+      <c r="D9" s="14">
+        <v>194.70989145721396</v>
+      </c>
+      <c r="E9" s="19">
+        <v>3</v>
+      </c>
+      <c r="F9" s="14">
+        <v>2593.469402473766</v>
+      </c>
+      <c r="G9" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="17">
+        <v>507.12800355799163</v>
+      </c>
+      <c r="C10" s="18">
+        <v>6</v>
+      </c>
+      <c r="D10" s="14">
+        <v>368.78703737093264</v>
+      </c>
+      <c r="E10" s="19">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14">
+        <v>875.91504092892433</v>
+      </c>
+      <c r="G10" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="17">
+        <v>4047.185460315171</v>
+      </c>
+      <c r="C11" s="18">
+        <v>24</v>
+      </c>
+      <c r="D11" s="14">
+        <v>1360.4863339463657</v>
+      </c>
+      <c r="E11" s="19">
+        <v>14</v>
+      </c>
+      <c r="F11" s="14">
+        <v>5407.6717942615369</v>
+      </c>
+      <c r="G11" s="19">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="B20" s="9">
+        <v>2018</v>
+      </c>
+      <c r="C20" s="22">
+        <v>2019</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="20">
+        <f>SUMIFS(data!$E$2:$E$39,data!A2:A39,Pivot!A21,data!F2:F39,Pivot!B20)</f>
+        <v>168.00692365944252</v>
+      </c>
+      <c r="C21" s="20">
+        <f>SUMIFS(data!$E$2:$E$39,data!$A$2:$A$39,Pivot!A21,data!$F$2:$F$39,Pivot!$C$20)</f>
+        <v>200.6171141802796</v>
+      </c>
+      <c r="D21" s="21">
+        <f>B21+C21</f>
+        <v>368.62403783972212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="20">
+        <f>SUMIFS(data!$E$2:$E$39,data!A2:A39,Pivot!A22,data!F2:F39,Pivot!B20)</f>
+        <v>902.13118892214493</v>
+      </c>
+      <c r="C22" s="20">
+        <f>SUMIFS(data!$E$2:$E$39,data!$A$2:$A$39,Pivot!A22,data!$F$2:$F$39,Pivot!$C$20)</f>
+        <v>562.87788636063124</v>
+      </c>
+      <c r="D22" s="21">
+        <f t="shared" ref="D22:D25" si="0">B22+C22</f>
+        <v>1465.0090752827762</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="20">
+        <f>SUMIFS(data!$E$2:$E$39,data!A2:A39,Pivot!A23,data!F2:F39,Pivot!B20)</f>
+        <v>71.15983315903982</v>
+      </c>
+      <c r="C23" s="20">
+        <f>SUMIFS(data!$E$2:$E$39,data!$A$2:$A$39,Pivot!A23,data!$F$2:$F$39,Pivot!$C$20)</f>
+        <v>33.494404577308188</v>
+      </c>
+      <c r="D23" s="21">
+        <f t="shared" si="0"/>
+        <v>104.65423773634801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="20">
+        <f>SUMIFS(data!$E$2:$E$39,data!A2:A39,Pivot!A24,data!F2:F39,Pivot!B20)</f>
+        <v>2398.7595110165521</v>
+      </c>
+      <c r="C24" s="20">
+        <f>SUMIFS(data!$E$2:$E$39,data!$A$2:$A$39,Pivot!A24,data!$F$2:$F$39,Pivot!$C$20)</f>
+        <v>194.70989145721396</v>
+      </c>
+      <c r="D24" s="21">
+        <f t="shared" si="0"/>
+        <v>2593.469402473766</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="20">
+        <f>SUMIFS(data!$E$2:$E$39,data!A2:A39,Pivot!A25,data!F2:F39,Pivot!B20)</f>
+        <v>507.12800355799163</v>
+      </c>
+      <c r="C25" s="20">
+        <f>SUMIFS(data!$E$2:$E$39,data!$A$2:$A$39,Pivot!A25,data!$F$2:$F$39,Pivot!$C$20)</f>
+        <v>368.78703737093264</v>
+      </c>
+      <c r="D25" s="21">
+        <f t="shared" si="0"/>
+        <v>875.91504092892433</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="21">
+        <f>SUM(B21:B25)</f>
+        <v>4047.185460315171</v>
+      </c>
+      <c r="C26" s="21">
+        <f t="shared" ref="C26:D26" si="1">SUM(C21:C25)</f>
+        <v>1360.4863339463657</v>
+      </c>
+      <c r="D26" s="21">
+        <f t="shared" si="1"/>
+        <v>5407.6717942615369</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr applyStyles="1"/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
+    <col min="2" max="2" width="26.796875" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="42" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="60" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.59765625" customWidth="1"/>
+    <col min="6" max="6" width="14.3984375" customWidth="1"/>
+    <col min="7" max="7" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="33" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="35" max="41" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="43" max="59" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="34.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -775,8 +1753,11 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -792,8 +1773,11 @@
       <c r="E2" s="6">
         <v>140.35435673674468</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F2" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -809,8 +1793,11 @@
       <c r="E3" s="6">
         <v>45.07590782878367</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F3" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -826,8 +1813,11 @@
       <c r="E4" s="6">
         <v>36.06</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F4" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -843,8 +1833,11 @@
       <c r="E5" s="6">
         <v>16.45571141802796</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F5" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -860,8 +1853,11 @@
       <c r="E6" s="6">
         <v>24.202757443534914</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F6" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -877,8 +1873,11 @@
       <c r="E7" s="6">
         <v>106.47530441263088</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F7" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -894,8 +1893,11 @@
       <c r="E8" s="6">
         <v>237.14735614775282</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F8" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -911,8 +1913,11 @@
       <c r="E9" s="6">
         <v>145.19250417703412</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F9" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -928,8 +1933,11 @@
       <c r="E10" s="6">
         <v>55.94220667604246</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F10" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -945,8 +1953,11 @@
       <c r="E11" s="6">
         <v>84.213816066255575</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F11" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -962,8 +1973,11 @@
       <c r="E12" s="6">
         <v>435.5775125311024</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F12" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -979,8 +1993,11 @@
       <c r="E13" s="6">
         <v>203.268303823639</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F13" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -996,8 +2013,11 @@
       <c r="E14" s="6">
         <v>300.06130323464714</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F14" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1013,8 +2033,11 @@
       <c r="E15" s="6">
         <v>3.6060726263026939</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F15" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1030,8 +2053,11 @@
       <c r="E16" s="6">
         <v>77.891168728138183</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F16" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -1047,8 +2073,11 @@
       <c r="E17" s="6">
         <v>193.39367494861347</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F17" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -1064,8 +2093,11 @@
       <c r="E18" s="6">
         <v>1254.4805452381811</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F18" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16">
       <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
@@ -1081,8 +2113,11 @@
       <c r="E19" s="6">
         <v>38.945584364069092</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F19" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1098,8 +2133,11 @@
       <c r="E20" s="6">
         <v>93.036673758609496</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F20" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16">
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
@@ -1115,8 +2153,11 @@
       <c r="E21" s="6">
         <v>62.727633334535362</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F21" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
@@ -1132,8 +2173,11 @@
       <c r="E22" s="6">
         <v>36.595627035928501</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F22" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -1149,8 +2193,11 @@
       <c r="E23" s="6">
         <v>365.98031084346042</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F23" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16">
       <c r="A24" s="3" t="s">
         <v>14</v>
       </c>
@@ -1166,8 +2213,11 @@
       <c r="E24" s="6">
         <v>470.41818422223025</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F24" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
@@ -1183,8 +2233,11 @@
       <c r="E25" s="6">
         <v>5.5233012392869592</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F25" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -1200,8 +2253,11 @@
       <c r="E26" s="6">
         <v>25.170386931592802</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F26" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
@@ -1217,8 +2273,11 @@
       <c r="E27" s="6">
         <v>20.332239491303355</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F27" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16">
       <c r="A28" s="3" t="s">
         <v>15</v>
       </c>
@@ -1234,8 +2293,11 @@
       <c r="E28" s="6">
         <v>5.613453054944527</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F28" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
@@ -1251,8 +2313,11 @@
       <c r="E29" s="6">
         <v>9.4959912492637599</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F29" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16">
       <c r="A30" s="3" t="s">
         <v>15</v>
       </c>
@@ -1268,8 +2333,11 @@
       <c r="E30" s="6">
         <v>7.5487120310603055</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F30" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
@@ -1285,8 +2353,11 @@
       <c r="E31" s="6">
         <v>18.390970394143739</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F31" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16">
       <c r="A32" s="3" t="s">
         <v>15</v>
       </c>
@@ -1302,8 +2373,11 @@
       <c r="E32" s="6">
         <v>12.579183344752563</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F32" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16">
       <c r="A33" s="3" t="s">
         <v>16</v>
       </c>
@@ -1319,8 +2393,11 @@
       <c r="E33" s="6">
         <v>132.87175603716659</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F33" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16">
       <c r="A34" s="3" t="s">
         <v>16</v>
       </c>
@@ -1336,8 +2413,11 @@
       <c r="E34" s="6">
         <v>86.113014316108334</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F34" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16">
       <c r="A35" s="3" t="s">
         <v>16</v>
       </c>
@@ -1353,8 +2433,11 @@
       <c r="E35" s="6">
         <v>368.78703737093264</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F35" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="16">
       <c r="A36" s="3" t="s">
         <v>16</v>
       </c>
@@ -1370,8 +2453,11 @@
       <c r="E36" s="6">
         <v>87.549433245585561</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F36" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="16">
       <c r="A37" s="3" t="s">
         <v>16</v>
       </c>
@@ -1387,8 +2473,11 @@
       <c r="E37" s="6">
         <v>119.75166179846862</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F37" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="16">
       <c r="A38" s="3" t="s">
         <v>16</v>
       </c>
@@ -1404,8 +2493,11 @@
       <c r="E38" s="6">
         <v>47.708340845984637</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F38" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="16">
       <c r="A39" s="7" t="s">
         <v>16</v>
       </c>
@@ -1420,6 +2512,9 @@
       </c>
       <c r="E39" s="8">
         <v>33.133797314677921</v>
+      </c>
+      <c r="F39" s="7">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>